<commit_message>
Added analysis for ratio and pessimistic functions
</commit_message>
<xml_diff>
--- a/heuristic-analysis/Analysis Results.xlsx
+++ b/heuristic-analysis/Analysis Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="22980" windowHeight="9024" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="24" windowWidth="22980" windowHeight="9024"/>
   </bookViews>
   <sheets>
     <sheet name="Ratio Evaluation Function" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,6 @@
     <sheet name="3 Feature GA Results" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -258,6 +257,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -290,12 +295,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -451,11 +450,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="179523520"/>
-        <c:axId val="179524096"/>
+        <c:axId val="130967808"/>
+        <c:axId val="130968384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="179523520"/>
+        <c:axId val="130967808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -484,12 +483,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="179524096"/>
+        <c:crossAx val="130968384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="179524096"/>
+        <c:axId val="130968384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -519,7 +518,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="179523520"/>
+        <c:crossAx val="130967808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -551,6 +550,26 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Win Rate of Agent Over Trials</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -667,26 +686,45 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="179525824"/>
-        <c:axId val="179526400"/>
+        <c:axId val="130970112"/>
+        <c:axId val="130970688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="179525824"/>
+        <c:axId val="130970112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Trial</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="179526400"/>
+        <c:crossAx val="130970688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="179526400"/>
+        <c:axId val="130970688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -694,11 +732,30 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Win Rate (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="179525824"/>
+        <c:crossAx val="130970112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -745,7 +802,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1170,11 +1226,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="42544640"/>
-        <c:axId val="199483968"/>
+        <c:axId val="131516416"/>
+        <c:axId val="130972416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42544640"/>
+        <c:axId val="131516416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1196,13 +1252,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199483968"/>
+        <c:crossAx val="130972416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1210,7 +1265,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199483968"/>
+        <c:axId val="130972416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="50"/>
@@ -1234,14 +1289,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42544640"/>
+        <c:crossAx val="131516416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1421,11 +1475,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="152930816"/>
-        <c:axId val="126676928"/>
+        <c:axId val="191286784"/>
+        <c:axId val="191627840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="152930816"/>
+        <c:axId val="191286784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1453,7 +1507,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126676928"/>
+        <c:crossAx val="191627840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1461,7 +1515,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126676928"/>
+        <c:axId val="191627840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="50"/>
@@ -1492,7 +1546,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152930816"/>
+        <c:crossAx val="191286784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1554,15 +1608,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>167640</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1943,8 +1997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1954,30 +2008,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:9" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -2101,7 +2155,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2110,63 +2164,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -2300,30 +2354,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:19" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="O3" s="4" t="s">
@@ -2484,12 +2538,12 @@
       <c r="B14">
         <v>68.599999999999994</v>
       </c>
-      <c r="O14" s="17" t="s">
+      <c r="O14" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="19"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="21"/>
       <c r="S14" s="3"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
@@ -2500,10 +2554,10 @@
       <c r="B15">
         <v>64.3</v>
       </c>
-      <c r="O15" s="20"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="24"/>
       <c r="S15" s="3"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
@@ -2514,10 +2568,10 @@
       <c r="B16">
         <v>57.1</v>
       </c>
-      <c r="O16" s="20"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="24"/>
       <c r="S16" s="3"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
@@ -2528,10 +2582,10 @@
       <c r="B17">
         <v>58.6</v>
       </c>
-      <c r="O17" s="20"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="24"/>
       <c r="S17" s="3"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
@@ -2542,10 +2596,10 @@
       <c r="B18">
         <v>65.7</v>
       </c>
-      <c r="O18" s="20"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="24"/>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
       <c r="U18" s="2"/>
@@ -2558,10 +2612,10 @@
       <c r="B19">
         <v>61.4</v>
       </c>
-      <c r="O19" s="20"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="24"/>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
@@ -2574,10 +2628,10 @@
       <c r="B20">
         <v>65.7</v>
       </c>
-      <c r="O20" s="20"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="24"/>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
@@ -2590,10 +2644,10 @@
       <c r="B21">
         <v>67.099999999999994</v>
       </c>
-      <c r="O21" s="20"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="24"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
@@ -2606,10 +2660,10 @@
       <c r="B22">
         <v>65.7</v>
       </c>
-      <c r="O22" s="20"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="24"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
@@ -2622,10 +2676,10 @@
       <c r="B23">
         <v>67.099999999999994</v>
       </c>
-      <c r="O23" s="20"/>
-      <c r="P23" s="21"/>
-      <c r="Q23" s="21"/>
-      <c r="R23" s="22"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="24"/>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
@@ -2638,10 +2692,10 @@
       <c r="B24">
         <v>64.3</v>
       </c>
-      <c r="O24" s="20"/>
-      <c r="P24" s="21"/>
-      <c r="Q24" s="21"/>
-      <c r="R24" s="22"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="24"/>
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
@@ -2654,10 +2708,10 @@
       <c r="B25">
         <v>55.7</v>
       </c>
-      <c r="O25" s="23"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="27"/>
       <c r="U25" s="2"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
@@ -3629,7 +3683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
@@ -3641,30 +3695,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:18" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="O3" s="4" t="s">
@@ -3767,7 +3821,7 @@
       <c r="O10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="P10" s="27">
+      <c r="P10" s="16">
         <v>-2.2911281281999201</v>
       </c>
     </row>
@@ -3779,8 +3833,8 @@
       <c r="B11">
         <v>60</v>
       </c>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -3790,12 +3844,12 @@
       <c r="B12">
         <v>68.599999999999994</v>
       </c>
-      <c r="O12" s="17" t="s">
+      <c r="O12" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="19"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="21"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -3805,10 +3859,10 @@
       <c r="B13">
         <v>65.7</v>
       </c>
-      <c r="O13" s="20"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="22"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="24"/>
     </row>
     <row r="14" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -3818,10 +3872,10 @@
       <c r="B14">
         <v>64.3</v>
       </c>
-      <c r="O14" s="20"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="24"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -3831,10 +3885,10 @@
       <c r="B15">
         <v>65.7</v>
       </c>
-      <c r="O15" s="20"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="24"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -3844,10 +3898,10 @@
       <c r="B16">
         <v>61.4</v>
       </c>
-      <c r="O16" s="20"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="24"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -3857,10 +3911,10 @@
       <c r="B17">
         <v>61.4</v>
       </c>
-      <c r="O17" s="20"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="24"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
@@ -3870,10 +3924,10 @@
       <c r="B18">
         <v>64.3</v>
       </c>
-      <c r="O18" s="20"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="24"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
@@ -3883,10 +3937,10 @@
       <c r="B19">
         <v>58.6</v>
       </c>
-      <c r="O19" s="20"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="24"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
@@ -3896,10 +3950,10 @@
       <c r="B20">
         <v>62.9</v>
       </c>
-      <c r="O20" s="20"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="24"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21">
@@ -3909,10 +3963,10 @@
       <c r="B21">
         <v>62.9</v>
       </c>
-      <c r="O21" s="20"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="24"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -3922,10 +3976,10 @@
       <c r="B22">
         <v>62.9</v>
       </c>
-      <c r="O22" s="20"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="24"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23">
@@ -3935,10 +3989,10 @@
       <c r="B23">
         <v>54.3</v>
       </c>
-      <c r="O23" s="23"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="25"/>
+      <c r="O23" s="25"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="26"/>
+      <c r="R23" s="27"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24">

</xml_diff>

<commit_message>
Updated Analysis Results Excel Chart with Experiment Data
</commit_message>
<xml_diff>
--- a/heuristic-analysis/Analysis Results.xlsx
+++ b/heuristic-analysis/Analysis Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="22980" windowHeight="9024"/>
+    <workbookView xWindow="0" yWindow="24" windowWidth="22980" windowHeight="9024" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Ratio Evaluation Function" sheetId="1" r:id="rId1"/>
@@ -450,11 +450,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="130967808"/>
-        <c:axId val="130968384"/>
+        <c:axId val="170576128"/>
+        <c:axId val="170576704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="130967808"/>
+        <c:axId val="170576128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -483,12 +483,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130968384"/>
+        <c:crossAx val="170576704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="130968384"/>
+        <c:axId val="170576704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -518,7 +518,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130967808"/>
+        <c:crossAx val="170576128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -570,7 +570,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -686,11 +685,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="130970112"/>
-        <c:axId val="130970688"/>
+        <c:axId val="170578432"/>
+        <c:axId val="170579008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="130970112"/>
+        <c:axId val="170578432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -712,19 +711,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130970688"/>
+        <c:crossAx val="170579008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="130970688"/>
+        <c:axId val="170579008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -748,14 +746,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130970112"/>
+        <c:crossAx val="170578432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -802,6 +799,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1226,11 +1224,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="131516416"/>
-        <c:axId val="130972416"/>
+        <c:axId val="190674944"/>
+        <c:axId val="170580736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="131516416"/>
+        <c:axId val="190674944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1252,12 +1250,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130972416"/>
+        <c:crossAx val="170580736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1265,7 +1264,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="130972416"/>
+        <c:axId val="170580736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="50"/>
@@ -1289,13 +1288,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131516416"/>
+        <c:crossAx val="190674944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1370,12 +1370,402 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'3 Feature GA Results'!$A$5:$A$131</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="127"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>127</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'3 Feature GA Results'!$B$5:$B$32</c:f>
+              <c:f>'3 Feature GA Results'!$B$5:$B$131</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="127"/>
                 <c:pt idx="0">
                   <c:v>70</c:v>
                 </c:pt>
@@ -1459,6 +1849,303 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>67.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>68.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>77.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>67.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>65.7</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>55.7</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>65.7</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>65.7</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>68.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>68.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>68.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>67.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>67.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>65.7</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>54.3</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>65.7</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>67.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>65.7</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>67.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>67.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>65.7</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>67.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>67.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>68.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>67.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>64.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1475,11 +2162,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="191286784"/>
-        <c:axId val="191627840"/>
+        <c:axId val="190042624"/>
+        <c:axId val="191038016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="191286784"/>
+        <c:axId val="190042624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1504,10 +2191,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191627840"/>
+        <c:crossAx val="191038016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1515,7 +2203,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191627840"/>
+        <c:axId val="191038016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="50"/>
@@ -1534,7 +2222,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-CA"/>
-                  <a:t>Win Rate</a:t>
+                  <a:t>Win Rate (%)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1546,16 +2234,11 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191286784"/>
+        <c:crossAx val="190042624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1997,7 +2680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -2342,7 +3025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U131"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:R25"/>
     </sheetView>
   </sheetViews>
@@ -3681,10 +4364,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R32"/>
+  <dimension ref="A1:R131"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3725,8 +4408,8 @@
         <v>5</v>
       </c>
       <c r="P3" s="5">
-        <f>MAX(B5:B32)</f>
-        <v>72.900000000000006</v>
+        <f>MAX(B5:B131)</f>
+        <v>77.099999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -3740,8 +4423,8 @@
         <v>6</v>
       </c>
       <c r="P4" s="7">
-        <f>AVERAGE(B5:B32)</f>
-        <v>63.935714285714297</v>
+        <f>AVERAGE(B5:B131)</f>
+        <v>63.2417322834646</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -3755,7 +4438,7 @@
         <v>7</v>
       </c>
       <c r="P5" s="9">
-        <v>-0.23019999999999999</v>
+        <v>-1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -3769,7 +4452,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f t="shared" ref="A7:A32" si="0">A6+1</f>
+        <f t="shared" ref="A7:A70" si="0">A6+1</f>
         <v>3</v>
       </c>
       <c r="B7">
@@ -3792,7 +4475,7 @@
         <v>13</v>
       </c>
       <c r="P8" s="13">
-        <v>3.49506388279109</v>
+        <v>5.6265145439628403</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -3807,7 +4490,7 @@
         <v>14</v>
       </c>
       <c r="P9" s="13">
-        <v>12.079479934986299</v>
+        <v>2.1318059635578499</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -3822,7 +4505,7 @@
         <v>15</v>
       </c>
       <c r="P10" s="16">
-        <v>-2.2911281281999201</v>
+        <v>-1.2009211458089299</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -4073,6 +4756,897 @@
       </c>
       <c r="B32">
         <v>61.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B33">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B34">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B36">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B37">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B38">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B39">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B40">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B41">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B42">
+        <v>68.599999999999994</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B43">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B44">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B45">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B46">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B47">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B48">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B49">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B50">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B51">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B52">
+        <v>77.099999999999994</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B53">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B54">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B55">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B56">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B57">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B58">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B59">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B60">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B61">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B62">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B63">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B64">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B65">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B66">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B67">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B68">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B69">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="B70">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <f t="shared" ref="A71:A134" si="1">A70+1</f>
+        <v>67</v>
+      </c>
+      <c r="B71">
+        <v>55.7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="B72">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="B73">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="B74">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="B75">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="B76">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="B77">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="B78">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="B79">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="B80">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="B81">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="B82">
+        <v>68.599999999999994</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="B83">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="B84">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="B85">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="B86">
+        <v>68.599999999999994</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="B87">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="B88">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="B89">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="B90">
+        <v>68.599999999999994</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="B91">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="B92">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="B93">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="B94">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="B95">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="B96">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="B97">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="B98">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="B99">
+        <v>54.3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="B100">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="B101">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="B102">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="B103">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="B104">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+      <c r="B105">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="B106">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="B107">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="B108">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="B109">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="B110">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="B111">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="B112">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="B113">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="B114">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="B115">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="B116">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="B117">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="B118">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
+      <c r="B119">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="B120">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="B121">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="B122">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+      <c r="B123">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="B124">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="B125">
+        <v>68.599999999999994</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="B126">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+      <c r="B127">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="B128">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="B129">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+      <c r="B130">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
+      <c r="B131">
+        <v>64.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 3 Feature GA Tab
</commit_message>
<xml_diff>
--- a/heuristic-analysis/Analysis Results.xlsx
+++ b/heuristic-analysis/Analysis Results.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="22980" windowHeight="9024" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="24" windowWidth="22980" windowHeight="9024" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ratio Evaluation Function" sheetId="1" r:id="rId1"/>
     <sheet name="Pessimistic Evaluation Function" sheetId="4" r:id="rId2"/>
-    <sheet name="5 Feature GA Results" sheetId="2" r:id="rId3"/>
+    <sheet name="GA Evaluation Function" sheetId="5" r:id="rId3"/>
     <sheet name="3 Feature GA Results" sheetId="3" r:id="rId4"/>
+    <sheet name="5 Feature GA Results" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>Std Dev</t>
   </si>
@@ -102,6 +103,33 @@
   </si>
   <si>
     <t>The following table shows the results of a 3-feature heuristic evaluation function trained using a genetic algorithm. Specifically, the following table only depicts the best agent per generation, the best performing agent agent overall, and the trend in win-rate over time. The performance of the agents is determined solely by its win rate.</t>
+  </si>
+  <si>
+    <t>Heuristic Analysis for the 3 Feature Genetic Algorithm Evaluation Function</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A Note About the Features:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The five features selected for the model was as follows:
+1) improved_score() provided by Udacity
+2) open_move_score() provided by Udacity
+3) center_score() provided by Udacity
+Note that some features overlap above, and that was intentionally done to observe the effects of having overlap in the model.</t>
+    </r>
+  </si>
+  <si>
+    <t>The following table shows the win rate, mean, and standard deviation of the performance of an Isolation game-playing agent using the 3 Feature Genetic Algorithm with parameters that gave it the maximum win rate during training. More information can be found in 3 Feature GA Results.
+A 5 Feature Genetic Algorithm was also experimented with; however, its results were not as strong as the 3 Feature Genetic Algorithm</t>
   </si>
 </sst>
 </file>
@@ -225,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -295,6 +323,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -450,11 +481,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="170576128"/>
         <c:axId val="170576704"/>
+        <c:axId val="170577280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="170576128"/>
+        <c:axId val="170576704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -483,12 +514,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170576704"/>
+        <c:crossAx val="170577280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="170576704"/>
+        <c:axId val="170577280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -518,7 +549,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170576128"/>
+        <c:crossAx val="170576704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -570,6 +601,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -685,11 +717,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="170578432"/>
         <c:axId val="170579008"/>
+        <c:axId val="170579584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="170578432"/>
+        <c:axId val="170579008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -711,563 +743,22 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170579008"/>
+        <c:crossAx val="170579584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="170579008"/>
+        <c:axId val="170579584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-CA"/>
-                  <a:t>Win Rate (%)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170578432"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-CA"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Win Rate over Generation</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'5 Feature GA Results'!$B$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Win Rate(%)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>'5 Feature GA Results'!$B$5:$B$131</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="127"/>
-                <c:pt idx="0">
-                  <c:v>54.3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>57.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>65.7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>57.1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>58.6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>68.599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>57.1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>58.6</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>65.7</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>65.7</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>67.099999999999994</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>65.7</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>67.099999999999994</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>55.7</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>65.7</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>62.9</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>62.9</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>55.7</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>65.7</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>58.6</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>62.9</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>55.7</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>58.6</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>58.6</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>57.1</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>62.9</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>62.9</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>58.6</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>65.7</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>65.7</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>68.599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>62.9</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>68.599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>62.9</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>68.599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>62.9</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>68.599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>72.900000000000006</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>65.7</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>68.599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>65.7</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>62.9</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>67.099999999999994</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>57.1</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>65.7</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>57.1</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>58.6</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>58.6</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>68.599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>55.7</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>57.1</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>62.9</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>62.9</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>55.7</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>67.099999999999994</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>71.400000000000006</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>62.9</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>67.099999999999994</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>55.7</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>68.599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>64.3</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>71.400000000000006</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>58.6</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>67.099999999999994</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>61.4</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>68.599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>64.3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="190674944"/>
-        <c:axId val="170580736"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="190674944"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-CA"/>
-                  <a:t>Generation</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170580736"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="170580736"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="50"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1295,9 +786,9 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190674944"/>
+        <c:crossAx val="170579008"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -1312,7 +803,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-CA"/>
@@ -2162,11 +1653,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190042624"/>
-        <c:axId val="191038016"/>
+        <c:axId val="193085952"/>
+        <c:axId val="170581312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190042624"/>
+        <c:axId val="193085952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2195,7 +1686,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191038016"/>
+        <c:crossAx val="170581312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2203,7 +1694,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191038016"/>
+        <c:axId val="170581312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="50"/>
@@ -2234,7 +1725,547 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190042624"/>
+        <c:crossAx val="193085952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Win Rate over Generation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'5 Feature GA Results'!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Win Rate(%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'5 Feature GA Results'!$B$5:$B$131</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="127"/>
+                <c:pt idx="0">
+                  <c:v>54.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>68.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65.7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>65.7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>67.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>65.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>67.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>55.7</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>65.7</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>55.7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>65.7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>55.7</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>65.7</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>65.7</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>68.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>68.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>68.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>72.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>65.7</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>68.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>65.7</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>67.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>65.7</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>68.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>55.7</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>55.7</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>67.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>71.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>67.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>55.7</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>68.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>71.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>67.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>68.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>64.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="193088512"/>
+        <c:axId val="193135744"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="193088512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Generation</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="193135744"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="193135744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Win Rate (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="193088512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2326,19 +2357,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
+      <xdr:colOff>243840</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>7621</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2361,19 +2392,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
+      <xdr:colOff>312420</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:rowOff>152401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>7621</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2681,7 +2712,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2838,7 +2869,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B8" sqref="B8:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3022,6 +3053,1454 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5" spans="1:9" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R131"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+    </row>
+    <row r="2" spans="1:18" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="5">
+        <f>MAX(B5:B131)</f>
+        <v>77.099999999999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P4" s="7">
+        <f>AVERAGE(B5:B131)</f>
+        <v>63.2417322834646</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>70</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5" s="9">
+        <v>-1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f>A5+1</f>
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" ref="A7:A70" si="0">A6+1</f>
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P7" s="11"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="P8" s="13">
+        <v>5.6265145439628403</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="O9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="P9" s="13">
+        <v>2.1318059635578499</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>65.7</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="P10" s="16">
+        <v>-1.2009211458089299</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>60</v>
+      </c>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+    </row>
+    <row r="12" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="O12" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="21"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>65.7</v>
+      </c>
+      <c r="O13" s="22"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="24"/>
+    </row>
+    <row r="14" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>64.3</v>
+      </c>
+      <c r="O14" s="22"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="24"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>65.7</v>
+      </c>
+      <c r="O15" s="22"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="24"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>61.4</v>
+      </c>
+      <c r="O16" s="22"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="24"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>61.4</v>
+      </c>
+      <c r="O17" s="22"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="24"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>64.3</v>
+      </c>
+      <c r="O18" s="22"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="24"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>58.6</v>
+      </c>
+      <c r="O19" s="22"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="24"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>62.9</v>
+      </c>
+      <c r="O20" s="22"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="24"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>62.9</v>
+      </c>
+      <c r="O21" s="25"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="27"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>62.9</v>
+      </c>
+      <c r="O22" s="28"/>
+      <c r="P22" s="28"/>
+      <c r="Q22" s="28"/>
+      <c r="R22" s="28"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>54.3</v>
+      </c>
+      <c r="O23" s="28"/>
+      <c r="P23" s="28"/>
+      <c r="Q23" s="28"/>
+      <c r="R23" s="28"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B26">
+        <v>72.900000000000006</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B27">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B30">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B31">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B32">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B33">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B34">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B36">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B37">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B38">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B39">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B40">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B41">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B42">
+        <v>68.599999999999994</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B43">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B44">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B45">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B46">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B47">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B48">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B49">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B50">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B51">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B52">
+        <v>77.099999999999994</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B53">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B54">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B55">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B56">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B57">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B58">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B59">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B60">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B61">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B62">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B63">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B64">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B65">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B66">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B67">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B68">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B69">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="B70">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <f t="shared" ref="A71:A131" si="1">A70+1</f>
+        <v>67</v>
+      </c>
+      <c r="B71">
+        <v>55.7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="B72">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="B73">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="B74">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="B75">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="B76">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="B77">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="B78">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="B79">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="B80">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="B81">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="B82">
+        <v>68.599999999999994</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="B83">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="B84">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="B85">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="B86">
+        <v>68.599999999999994</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="B87">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="B88">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="B89">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="B90">
+        <v>68.599999999999994</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="B91">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="B92">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="B93">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="B94">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="B95">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="B96">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="B97">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="B98">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="B99">
+        <v>54.3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="B100">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="B101">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="B102">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="B103">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="B104">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+      <c r="B105">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="B106">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="B107">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="B108">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="B109">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="B110">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="B111">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="B112">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="B113">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="B114">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="B115">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="B116">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="B117">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="B118">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
+      <c r="B119">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="B120">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="B121">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="B122">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+      <c r="B123">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="B124">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="B125">
+        <v>68.599999999999994</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="B126">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+      <c r="B127">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="B128">
+        <v>67.099999999999994</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="B129">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+      <c r="B130">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
+      <c r="B131">
+        <v>64.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="O12:R21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U131"/>
   <sheetViews>
@@ -4360,1302 +5839,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R131"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-    </row>
-    <row r="2" spans="1:18" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="O3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="P3" s="5">
-        <f>MAX(B5:B131)</f>
-        <v>77.099999999999994</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P4" s="7">
-        <f>AVERAGE(B5:B131)</f>
-        <v>63.2417322834646</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>70</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P5" s="9">
-        <v>-1.7999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <f>A5+1</f>
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>67.099999999999994</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <f t="shared" ref="A7:A70" si="0">A6+1</f>
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>68.599999999999994</v>
-      </c>
-      <c r="O7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="P7" s="11"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>67.099999999999994</v>
-      </c>
-      <c r="O8" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="P8" s="13">
-        <v>5.6265145439628403</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>68.599999999999994</v>
-      </c>
-      <c r="O9" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="P9" s="13">
-        <v>2.1318059635578499</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B10">
-        <v>65.7</v>
-      </c>
-      <c r="O10" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="P10" s="16">
-        <v>-1.2009211458089299</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>60</v>
-      </c>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B12">
-        <v>68.599999999999994</v>
-      </c>
-      <c r="O12" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="21"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B13">
-        <v>65.7</v>
-      </c>
-      <c r="O13" s="22"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="24"/>
-    </row>
-    <row r="14" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <v>64.3</v>
-      </c>
-      <c r="O14" s="22"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="24"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B15">
-        <v>65.7</v>
-      </c>
-      <c r="O15" s="22"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="24"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B16">
-        <v>61.4</v>
-      </c>
-      <c r="O16" s="22"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="24"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B17">
-        <v>61.4</v>
-      </c>
-      <c r="O17" s="22"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="24"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B18">
-        <v>64.3</v>
-      </c>
-      <c r="O18" s="22"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="24"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B19">
-        <v>58.6</v>
-      </c>
-      <c r="O19" s="22"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="24"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B20">
-        <v>62.9</v>
-      </c>
-      <c r="O20" s="22"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="24"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B21">
-        <v>62.9</v>
-      </c>
-      <c r="O21" s="22"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="24"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B22">
-        <v>62.9</v>
-      </c>
-      <c r="O22" s="22"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="23"/>
-      <c r="R22" s="24"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B23">
-        <v>54.3</v>
-      </c>
-      <c r="O23" s="25"/>
-      <c r="P23" s="26"/>
-      <c r="Q23" s="26"/>
-      <c r="R23" s="27"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B24">
-        <v>64.3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B25">
-        <v>62.9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B26">
-        <v>72.900000000000006</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B27">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B28">
-        <v>64.3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B29">
-        <v>61.4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B30">
-        <v>64.3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B31">
-        <v>58.6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B32">
-        <v>61.4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B33">
-        <v>62.9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B34">
-        <v>61.4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B35">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B36">
-        <v>64.3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B37">
-        <v>61.4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B38">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="B39">
-        <v>58.6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="B40">
-        <v>67.099999999999994</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="B41">
-        <v>62.9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="B42">
-        <v>68.599999999999994</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="B43">
-        <v>61.4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="B44">
-        <v>64.3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="B45">
-        <v>62.9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="B46">
-        <v>64.3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="B47">
-        <v>64.3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B48">
-        <v>64.3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="B49">
-        <v>64.3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B50">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B51">
-        <v>62.9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="B52">
-        <v>77.099999999999994</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="B53">
-        <v>62.9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="B54">
-        <v>67.099999999999994</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="B55">
-        <v>58.6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="B56">
-        <v>62.9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="B57">
-        <v>65.7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="B58">
-        <v>61.4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="B59">
-        <v>64.3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="B60">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="B61">
-        <v>64.3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="B62">
-        <v>62.9</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="B63">
-        <v>62.9</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="B64">
-        <v>62.9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="B65">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="B66">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="B67">
-        <v>57.1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="B68">
-        <v>62.9</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="B69">
-        <v>64.3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="B70">
-        <v>61.4</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71">
-        <f t="shared" ref="A71:A134" si="1">A70+1</f>
-        <v>67</v>
-      </c>
-      <c r="B71">
-        <v>55.7</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72">
-        <f t="shared" si="1"/>
-        <v>68</v>
-      </c>
-      <c r="B72">
-        <v>61.4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73">
-        <f t="shared" si="1"/>
-        <v>69</v>
-      </c>
-      <c r="B73">
-        <v>61.4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="B74">
-        <v>64.3</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75">
-        <f t="shared" si="1"/>
-        <v>71</v>
-      </c>
-      <c r="B75">
-        <v>62.9</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76">
-        <f t="shared" si="1"/>
-        <v>72</v>
-      </c>
-      <c r="B76">
-        <v>65.7</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77">
-        <f t="shared" si="1"/>
-        <v>73</v>
-      </c>
-      <c r="B77">
-        <v>62.9</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78">
-        <f t="shared" si="1"/>
-        <v>74</v>
-      </c>
-      <c r="B78">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79">
-        <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
-      <c r="B79">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80">
-        <f t="shared" si="1"/>
-        <v>76</v>
-      </c>
-      <c r="B80">
-        <v>65.7</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81">
-        <f t="shared" si="1"/>
-        <v>77</v>
-      </c>
-      <c r="B81">
-        <v>62.9</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82">
-        <f t="shared" si="1"/>
-        <v>78</v>
-      </c>
-      <c r="B82">
-        <v>68.599999999999994</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83">
-        <f t="shared" si="1"/>
-        <v>79</v>
-      </c>
-      <c r="B83">
-        <v>57.1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="B84">
-        <v>61.4</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85">
-        <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="B85">
-        <v>62.9</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86">
-        <f t="shared" si="1"/>
-        <v>82</v>
-      </c>
-      <c r="B86">
-        <v>68.599999999999994</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87">
-        <f t="shared" si="1"/>
-        <v>83</v>
-      </c>
-      <c r="B87">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88">
-        <f t="shared" si="1"/>
-        <v>84</v>
-      </c>
-      <c r="B88">
-        <v>57.1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89">
-        <f t="shared" si="1"/>
-        <v>85</v>
-      </c>
-      <c r="B89">
-        <v>58.6</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90">
-        <f t="shared" si="1"/>
-        <v>86</v>
-      </c>
-      <c r="B90">
-        <v>68.599999999999994</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91">
-        <f t="shared" si="1"/>
-        <v>87</v>
-      </c>
-      <c r="B91">
-        <v>67.099999999999994</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92">
-        <f t="shared" si="1"/>
-        <v>88</v>
-      </c>
-      <c r="B92">
-        <v>67.099999999999994</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93">
-        <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="B93">
-        <v>65.7</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94">
-        <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="B94">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95">
-        <f t="shared" si="1"/>
-        <v>91</v>
-      </c>
-      <c r="B95">
-        <v>61.4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96">
-        <f t="shared" si="1"/>
-        <v>92</v>
-      </c>
-      <c r="B96">
-        <v>62.9</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97">
-        <f t="shared" si="1"/>
-        <v>93</v>
-      </c>
-      <c r="B97">
-        <v>58.6</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98">
-        <f t="shared" si="1"/>
-        <v>94</v>
-      </c>
-      <c r="B98">
-        <v>61.4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99">
-        <f t="shared" si="1"/>
-        <v>95</v>
-      </c>
-      <c r="B99">
-        <v>54.3</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100">
-        <f t="shared" si="1"/>
-        <v>96</v>
-      </c>
-      <c r="B100">
-        <v>65.7</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101">
-        <f t="shared" si="1"/>
-        <v>97</v>
-      </c>
-      <c r="B101">
-        <v>57.1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-      <c r="B102">
-        <v>64.3</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103">
-        <f t="shared" si="1"/>
-        <v>99</v>
-      </c>
-      <c r="B103">
-        <v>58.6</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="B104">
-        <v>67.099999999999994</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105">
-        <f t="shared" si="1"/>
-        <v>101</v>
-      </c>
-      <c r="B105">
-        <v>57.1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106">
-        <f t="shared" si="1"/>
-        <v>102</v>
-      </c>
-      <c r="B106">
-        <v>65.7</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107">
-        <f t="shared" si="1"/>
-        <v>103</v>
-      </c>
-      <c r="B107">
-        <v>61.4</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108">
-        <f t="shared" si="1"/>
-        <v>104</v>
-      </c>
-      <c r="B108">
-        <v>57.1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109">
-        <f t="shared" si="1"/>
-        <v>105</v>
-      </c>
-      <c r="B109">
-        <v>61.4</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110">
-        <f t="shared" si="1"/>
-        <v>106</v>
-      </c>
-      <c r="B110">
-        <v>64.3</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111">
-        <f t="shared" si="1"/>
-        <v>107</v>
-      </c>
-      <c r="B111">
-        <v>64.3</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112">
-        <f t="shared" si="1"/>
-        <v>108</v>
-      </c>
-      <c r="B112">
-        <v>67.099999999999994</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113">
-        <f t="shared" si="1"/>
-        <v>109</v>
-      </c>
-      <c r="B113">
-        <v>58.6</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114">
-        <f t="shared" si="1"/>
-        <v>110</v>
-      </c>
-      <c r="B114">
-        <v>67.099999999999994</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115">
-        <f t="shared" si="1"/>
-        <v>111</v>
-      </c>
-      <c r="B115">
-        <v>58.6</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116">
-        <f t="shared" si="1"/>
-        <v>112</v>
-      </c>
-      <c r="B116">
-        <v>62.9</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117">
-        <f t="shared" si="1"/>
-        <v>113</v>
-      </c>
-      <c r="B117">
-        <v>65.7</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118">
-        <f t="shared" si="1"/>
-        <v>114</v>
-      </c>
-      <c r="B118">
-        <v>62.9</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119">
-        <f t="shared" si="1"/>
-        <v>115</v>
-      </c>
-      <c r="B119">
-        <v>62.9</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120">
-        <f t="shared" si="1"/>
-        <v>116</v>
-      </c>
-      <c r="B120">
-        <v>64.3</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121">
-        <f t="shared" si="1"/>
-        <v>117</v>
-      </c>
-      <c r="B121">
-        <v>57.1</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122">
-        <f t="shared" si="1"/>
-        <v>118</v>
-      </c>
-      <c r="B122">
-        <v>67.099999999999994</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123">
-        <f t="shared" si="1"/>
-        <v>119</v>
-      </c>
-      <c r="B123">
-        <v>67.099999999999994</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124">
-        <f t="shared" si="1"/>
-        <v>120</v>
-      </c>
-      <c r="B124">
-        <v>61.4</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125">
-        <f t="shared" si="1"/>
-        <v>121</v>
-      </c>
-      <c r="B125">
-        <v>68.599999999999994</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A126">
-        <f t="shared" si="1"/>
-        <v>122</v>
-      </c>
-      <c r="B126">
-        <v>61.4</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127">
-        <f t="shared" si="1"/>
-        <v>123</v>
-      </c>
-      <c r="B127">
-        <v>64.3</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128">
-        <f t="shared" si="1"/>
-        <v>124</v>
-      </c>
-      <c r="B128">
-        <v>67.099999999999994</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129">
-        <f t="shared" si="1"/>
-        <v>125</v>
-      </c>
-      <c r="B129">
-        <v>61.4</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A130">
-        <f t="shared" si="1"/>
-        <v>126</v>
-      </c>
-      <c r="B130">
-        <v>58.6</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131">
-        <f t="shared" si="1"/>
-        <v>127</v>
-      </c>
-      <c r="B131">
-        <v>64.3</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="O12:R23"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added GA trial data
</commit_message>
<xml_diff>
--- a/heuristic-analysis/Analysis Results.xlsx
+++ b/heuristic-analysis/Analysis Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="22980" windowHeight="9024" activeTab="2"/>
+    <workbookView xWindow="11508" yWindow="-12" windowWidth="11544" windowHeight="9096"/>
   </bookViews>
   <sheets>
     <sheet name="Ratio Evaluation Function" sheetId="1" r:id="rId1"/>
@@ -291,6 +291,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -323,9 +326,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -481,11 +481,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="170576704"/>
-        <c:axId val="170577280"/>
+        <c:axId val="155241856"/>
+        <c:axId val="155242432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="170576704"/>
+        <c:axId val="155241856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -514,12 +514,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170577280"/>
+        <c:crossAx val="155242432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="170577280"/>
+        <c:axId val="155242432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,7 +549,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170576704"/>
+        <c:crossAx val="155241856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -717,11 +717,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="170579008"/>
-        <c:axId val="170579584"/>
+        <c:axId val="155244160"/>
+        <c:axId val="155244736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="170579008"/>
+        <c:axId val="155244160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -750,12 +750,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170579584"/>
+        <c:crossAx val="155244736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="170579584"/>
+        <c:axId val="155244736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -786,7 +786,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170579008"/>
+        <c:crossAx val="155244160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -838,7 +838,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1653,11 +1652,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="193085952"/>
-        <c:axId val="170581312"/>
+        <c:axId val="199377408"/>
+        <c:axId val="198565888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="193085952"/>
+        <c:axId val="199377408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1679,14 +1678,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170581312"/>
+        <c:crossAx val="198565888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1694,7 +1692,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170581312"/>
+        <c:axId val="198565888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="50"/>
@@ -1718,14 +1716,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193085952"/>
+        <c:crossAx val="199377408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2196,11 +2193,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="193088512"/>
-        <c:axId val="193135744"/>
+        <c:axId val="199379968"/>
+        <c:axId val="198567616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="193088512"/>
+        <c:axId val="199379968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2227,7 +2224,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193135744"/>
+        <c:crossAx val="198567616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2235,7 +2232,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="193135744"/>
+        <c:axId val="198567616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="50"/>
@@ -2265,7 +2262,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193088512"/>
+        <c:crossAx val="199379968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2711,8 +2708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2722,30 +2719,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -2849,8 +2846,8 @@
         <v>0</v>
       </c>
       <c r="B17">
-        <f>_xlfn.STDEV.P(B5:B14)</f>
-        <v>5.1453765654225938</v>
+        <f>_xlfn.STDEV.S(B5:B14)</f>
+        <v>5.4237031219965912</v>
       </c>
     </row>
   </sheetData>
@@ -2869,7 +2866,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B17"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2878,63 +2875,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -3038,8 +3035,8 @@
         <v>0</v>
       </c>
       <c r="B20">
-        <f>_xlfn.STDEV.P(B8:B17)</f>
-        <v>2.8596503282744208</v>
+        <f>_xlfn.STDEV.S(B8:B17)</f>
+        <v>3.014336116331791</v>
       </c>
     </row>
   </sheetData>
@@ -3056,8 +3053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3066,63 +3063,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -3136,60 +3133,98 @@
       <c r="A8">
         <v>1</v>
       </c>
+      <c r="B8">
+        <v>60</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
+      <c r="B9">
+        <v>70</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
+      <c r="B10">
+        <v>57.1</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
+      <c r="B11">
+        <v>64.3</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>60</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
+      <c r="B13">
+        <v>58.6</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
+      <c r="B14">
+        <v>58.6</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8</v>
       </c>
+      <c r="B15">
+        <v>60</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>62.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>52.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <f>AVERAGE(B8:B17)</f>
+        <v>60.44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B20">
+        <f>_xlfn.STDEV.S(B8:B17)</f>
+        <v>4.5668369797924688</v>
       </c>
     </row>
   </sheetData>
@@ -3218,30 +3253,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:18" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="O3" s="4" t="s">
@@ -3367,12 +3402,12 @@
       <c r="B12">
         <v>68.599999999999994</v>
       </c>
-      <c r="O12" s="19" t="s">
+      <c r="O12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="22"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -3382,10 +3417,10 @@
       <c r="B13">
         <v>65.7</v>
       </c>
-      <c r="O13" s="22"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="24"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="25"/>
     </row>
     <row r="14" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -3395,10 +3430,10 @@
       <c r="B14">
         <v>64.3</v>
       </c>
-      <c r="O14" s="22"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="24"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="25"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -3408,10 +3443,10 @@
       <c r="B15">
         <v>65.7</v>
       </c>
-      <c r="O15" s="22"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="24"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="25"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -3421,10 +3456,10 @@
       <c r="B16">
         <v>61.4</v>
       </c>
-      <c r="O16" s="22"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="24"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="25"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -3434,10 +3469,10 @@
       <c r="B17">
         <v>61.4</v>
       </c>
-      <c r="O17" s="22"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="24"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="25"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
@@ -3447,10 +3482,10 @@
       <c r="B18">
         <v>64.3</v>
       </c>
-      <c r="O18" s="22"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="24"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="25"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
@@ -3460,10 +3495,10 @@
       <c r="B19">
         <v>58.6</v>
       </c>
-      <c r="O19" s="22"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="24"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="25"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
@@ -3473,10 +3508,10 @@
       <c r="B20">
         <v>62.9</v>
       </c>
-      <c r="O20" s="22"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="24"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="25"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21">
@@ -3486,10 +3521,10 @@
       <c r="B21">
         <v>62.9</v>
       </c>
-      <c r="O21" s="25"/>
-      <c r="P21" s="26"/>
-      <c r="Q21" s="26"/>
-      <c r="R21" s="27"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="28"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -3499,10 +3534,10 @@
       <c r="B22">
         <v>62.9</v>
       </c>
-      <c r="O22" s="28"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="28"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23">
@@ -3512,10 +3547,10 @@
       <c r="B23">
         <v>54.3</v>
       </c>
-      <c r="O23" s="28"/>
-      <c r="P23" s="28"/>
-      <c r="Q23" s="28"/>
-      <c r="R23" s="28"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24">
@@ -4516,30 +4551,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:19" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="O3" s="4" t="s">
@@ -4700,12 +4735,12 @@
       <c r="B14">
         <v>68.599999999999994</v>
       </c>
-      <c r="O14" s="19" t="s">
+      <c r="O14" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="22"/>
       <c r="S14" s="3"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
@@ -4716,10 +4751,10 @@
       <c r="B15">
         <v>64.3</v>
       </c>
-      <c r="O15" s="22"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="24"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="25"/>
       <c r="S15" s="3"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
@@ -4730,10 +4765,10 @@
       <c r="B16">
         <v>57.1</v>
       </c>
-      <c r="O16" s="22"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="24"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="25"/>
       <c r="S16" s="3"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
@@ -4744,10 +4779,10 @@
       <c r="B17">
         <v>58.6</v>
       </c>
-      <c r="O17" s="22"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="24"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="25"/>
       <c r="S17" s="3"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
@@ -4758,10 +4793,10 @@
       <c r="B18">
         <v>65.7</v>
       </c>
-      <c r="O18" s="22"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="24"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="25"/>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
       <c r="U18" s="2"/>
@@ -4774,10 +4809,10 @@
       <c r="B19">
         <v>61.4</v>
       </c>
-      <c r="O19" s="22"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="24"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="25"/>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
@@ -4790,10 +4825,10 @@
       <c r="B20">
         <v>65.7</v>
       </c>
-      <c r="O20" s="22"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="24"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="25"/>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
@@ -4806,10 +4841,10 @@
       <c r="B21">
         <v>67.099999999999994</v>
       </c>
-      <c r="O21" s="22"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="24"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="25"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
@@ -4822,10 +4857,10 @@
       <c r="B22">
         <v>65.7</v>
       </c>
-      <c r="O22" s="22"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="23"/>
-      <c r="R22" s="24"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="25"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
@@ -4838,10 +4873,10 @@
       <c r="B23">
         <v>67.099999999999994</v>
       </c>
-      <c r="O23" s="22"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="R23" s="24"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="24"/>
+      <c r="R23" s="25"/>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
@@ -4854,10 +4889,10 @@
       <c r="B24">
         <v>64.3</v>
       </c>
-      <c r="O24" s="22"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="23"/>
-      <c r="R24" s="24"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="24"/>
+      <c r="R24" s="25"/>
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
@@ -4870,10 +4905,10 @@
       <c r="B25">
         <v>55.7</v>
       </c>
-      <c r="O25" s="25"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="27"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="27"/>
+      <c r="R25" s="28"/>
       <c r="U25" s="2"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added a bar graph to compare the performance of different heuristics
</commit_message>
<xml_diff>
--- a/heuristic-analysis/Analysis Results.xlsx
+++ b/heuristic-analysis/Analysis Results.xlsx
@@ -12,6 +12,7 @@
     <sheet name="GA Evaluation Function" sheetId="5" r:id="rId3"/>
     <sheet name="3 Feature GA Results" sheetId="3" r:id="rId4"/>
     <sheet name="5 Feature GA Results" sheetId="2" r:id="rId5"/>
+    <sheet name="Comparison of 3 Heuristics" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -481,11 +482,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="155241856"/>
-        <c:axId val="155242432"/>
+        <c:axId val="138047424"/>
+        <c:axId val="138048000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="155241856"/>
+        <c:axId val="138047424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -514,12 +515,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155242432"/>
+        <c:crossAx val="138048000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="155242432"/>
+        <c:axId val="138048000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,7 +550,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155241856"/>
+        <c:crossAx val="138047424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -601,7 +602,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -717,11 +717,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="155244160"/>
-        <c:axId val="155244736"/>
+        <c:axId val="138049728"/>
+        <c:axId val="138050304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="155244160"/>
+        <c:axId val="138049728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,19 +743,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155244736"/>
+        <c:crossAx val="138050304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="155244736"/>
+        <c:axId val="138050304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -779,14 +778,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155244160"/>
+        <c:crossAx val="138049728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -859,7 +857,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -975,11 +972,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="145273920"/>
-        <c:axId val="145273344"/>
+        <c:axId val="199090752"/>
+        <c:axId val="199091328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="145273920"/>
+        <c:axId val="199090752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1001,19 +998,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145273344"/>
+        <c:crossAx val="199091328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="145273344"/>
+        <c:axId val="199091328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1041,14 +1037,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145273920"/>
+        <c:crossAx val="199090752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1100,7 +1095,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1915,11 +1909,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="199377408"/>
-        <c:axId val="198565888"/>
+        <c:axId val="199578112"/>
+        <c:axId val="199093056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="199377408"/>
+        <c:axId val="199578112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1941,14 +1935,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198565888"/>
+        <c:crossAx val="199093056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1956,7 +1949,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198565888"/>
+        <c:axId val="199093056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="50"/>
@@ -1980,14 +1973,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199377408"/>
+        <c:crossAx val="199578112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2034,7 +2026,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2459,11 +2450,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="199379968"/>
-        <c:axId val="198567616"/>
+        <c:axId val="199580160"/>
+        <c:axId val="199094784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="199379968"/>
+        <c:axId val="199580160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2485,13 +2476,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="198567616"/>
+        <c:crossAx val="199094784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2499,10 +2489,381 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="198567616"/>
+        <c:axId val="199094784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Win Rate (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="199580160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Win Rate of Agent Over Trials</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ratio Evaluation Function</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Pessimistic Evaluation Function'!$A$8:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ratio Evaluation Function'!$B$5:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>55.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>71.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Pessimistic Evaluation Function</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Pessimistic Evaluation Function'!$A$8:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pessimistic Evaluation Function'!$B$8:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>51.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>56.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>58.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>57.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>GA Evaluation Function</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'GA Evaluation Function'!$B$8:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>58.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>62.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="200119808"/>
+        <c:axId val="199096512"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="200119808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Trial</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="199096512"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="199096512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2530,11 +2891,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199379968"/>
+        <c:crossAx val="200119808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2706,6 +3072,43 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>532600</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3169,7 +3572,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A7" sqref="A7:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3357,7 +3760,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A7" sqref="A7:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6178,4 +6581,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>